<commit_message>
Updated Poster mobile responsiveness on index.html
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,73 +463,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nifemi  Spectro</t>
+          <t>Mimi</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>09125662818</t>
+          <t>08035987700</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>spectrobana@gmail.com</t>
+          <t>smilingmiriam@gmail.com</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>2025-09-18T09:17:02.291922+00:00</t>
+          <t>2025-09-18T14:15:27.058764+00:00</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Test User</t>
+          <t>Nifemi  Spectro</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>09123456789</t>
+          <t>09125662818</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>test@example.com</t>
+          <t>spectrobana@gmail.com</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>2025-09-18T07:38:58.177023+00:00</t>
+          <t>2025-09-18T09:47:44.947181+00:00</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Test User</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>09123456789</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>test@example.com</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>2025-09-18T07:38:58.177023+00:00</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>ace</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>9136666787</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>ace@gmail.com</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="D5" t="n">
         <v>1</v>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>2025-09-18T07:32:43.04661+00:00</t>
         </is>

</xml_diff>